<commit_message>
Atualizações do dia 05/05
</commit_message>
<xml_diff>
--- a/Banco de Dados/Dicionário de Dados.xlsx
+++ b/Banco de Dados/Dicionário de Dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Downloads\SwiftieVerso\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B694B4-3080-4651-B1DA-3868F20055BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A739827-727F-4165-99A5-0A51FE8BDC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="110">
   <si>
     <t>Tabela</t>
   </si>
@@ -194,24 +194,6 @@
   </si>
   <si>
     <t>Identificador único do endereco</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>complemento</t>
-  </si>
-  <si>
-    <t>Numero do endereço</t>
-  </si>
-  <si>
-    <t>Complemento do endereço</t>
-  </si>
-  <si>
-    <t>logradouro</t>
-  </si>
-  <si>
-    <t>Logradouro do endereço</t>
   </si>
   <si>
     <t>Chave estrangeira referenciando o id da cidade</t>
@@ -596,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -619,11 +601,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -645,6 +664,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L76"/>
+  <dimension ref="B2:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,12 +1011,12 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
@@ -976,12 +1031,12 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
       <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
@@ -996,12 +1051,12 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
       <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1013,13 +1068,13 @@
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
       <c r="H5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1160,17 +1215,17 @@
       <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
       <c r="H19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1180,17 +1235,17 @@
       <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
       <c r="H20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1200,30 +1255,30 @@
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
       <c r="H21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
       <c r="H22" s="6" t="s">
         <v>7</v>
       </c>
@@ -1281,10 +1336,10 @@
         <v>14</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>13</v>
@@ -1298,10 +1353,10 @@
     </row>
     <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>13</v>
@@ -1310,13 +1365,13 @@
         <v>9</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>17</v>
@@ -1330,23 +1385,25 @@
     </row>
     <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="1">
-        <v>50</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="H26" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>17</v>
@@ -1359,29 +1416,14 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="1">
-        <v>200</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H27" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>9</v>
@@ -1391,26 +1433,11 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="H28" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>20</v>
@@ -1419,30 +1446,15 @@
         <v>11</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="H29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="I29" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>17</v>
@@ -1451,15 +1463,15 @@
         <v>50</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H30" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>17</v>
@@ -1473,10 +1485,10 @@
     </row>
     <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H31" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>13</v>
@@ -1485,15 +1497,15 @@
         <v>9</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H32" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>13</v>
@@ -1509,17 +1521,17 @@
       <c r="B36" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="C36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="16"/>
       <c r="H36" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -1529,17 +1541,17 @@
       <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="C37" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13"/>
       <c r="H37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
@@ -1549,30 +1561,30 @@
       <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="C38" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
       <c r="H38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
     </row>
     <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19"/>
       <c r="H39" s="6" t="s">
         <v>7</v>
       </c>
@@ -1615,10 +1627,10 @@
     </row>
     <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -1630,10 +1642,10 @@
         <v>14</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>13</v>
@@ -1642,15 +1654,15 @@
         <v>9</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -1659,13 +1671,13 @@
         <v>9</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="I42" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>13</v>
@@ -1674,15 +1686,15 @@
         <v>9</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -1694,10 +1706,10 @@
         <v>18</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>13</v>
@@ -1706,15 +1718,15 @@
         <v>9</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>17</v>
@@ -1730,17 +1742,17 @@
       <c r="B53" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="C53" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="16"/>
       <c r="H53" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -1750,17 +1762,17 @@
       <c r="B54" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="C54" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="13"/>
       <c r="H54" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
@@ -1770,12 +1782,12 @@
       <c r="B55" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
+      <c r="C55" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
       <c r="H55" s="2" t="s">
         <v>2</v>
       </c>
@@ -1787,13 +1799,13 @@
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="19"/>
       <c r="H56" s="6" t="s">
         <v>7</v>
       </c>
@@ -1836,10 +1848,10 @@
     </row>
     <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -1851,10 +1863,10 @@
         <v>14</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>13</v>
@@ -1871,7 +1883,7 @@
         <v>11</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>17</v>
@@ -1886,7 +1898,7 @@
         <v>11</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>17</v>
@@ -1900,10 +1912,10 @@
     </row>
     <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -1915,13 +1927,13 @@
         <v>18</v>
       </c>
       <c r="H60" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="K60" s="1">
         <v>5.2</v>
@@ -1932,13 +1944,13 @@
     </row>
     <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="E61" s="1">
         <v>5.2</v>
@@ -1949,10 +1961,10 @@
     </row>
     <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -1961,124 +1973,115 @@
         <v>9</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="13"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="13"/>
     </row>
     <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
+      <c r="B70" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="10"/>
     </row>
     <row r="71" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
+      <c r="D71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
+      <c r="B72" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B73" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B74" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D75" s="1" t="s">
+      <c r="B73" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>82</v>
+      <c r="E73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="C70:F70"/>
-    <mergeCell ref="C71:F71"/>
-    <mergeCell ref="C72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="I53:L53"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="I55:L55"/>
-    <mergeCell ref="H56:L56"/>
+  <mergeCells count="34">
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C37:F37"/>
     <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="H5:L5"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="C21:F21"/>
@@ -2087,14 +2090,21 @@
     <mergeCell ref="I20:L20"/>
     <mergeCell ref="I21:L21"/>
     <mergeCell ref="H22:L22"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="I53:L53"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="I55:L55"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C55:F55"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Atualização do dia 13/05
</commit_message>
<xml_diff>
--- a/Banco de Dados/Dicionário de Dados.xlsx
+++ b/Banco de Dados/Dicionário de Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Downloads\SwiftieVerso\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F0DC73-5AEC-409A-B217-4B4EA3FE4262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6462F1-71ED-4E6E-BE23-9CC7A9394247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14520" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="112">
   <si>
     <t>Tabela</t>
   </si>
@@ -235,12 +235,6 @@
   </si>
   <si>
     <t>Primeiro nome do usuário</t>
-  </si>
-  <si>
-    <t>fkCidade</t>
-  </si>
-  <si>
-    <t>Chave estrangeira referenciando o id da cidade</t>
   </si>
   <si>
     <t>sobrenome</t>
@@ -681,25 +675,13 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,6 +695,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,1118 +1131,1104 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="H3" s="5" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="H4" s="5" t="s">
+      <c r="C4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="6" t="s">
+      <c r="K7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="2">
         <v>45</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="2">
         <v>50</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="K9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="H19" s="5" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="H19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="H20" s="5" t="s">
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="H20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="H21" s="5" t="s">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="H21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="H22" s="2" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="H22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L24" s="6" t="s">
+      <c r="K24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="E25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="J25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="2">
         <v>20</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="H26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="I26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="J26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="2">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" s="2">
+        <v>11</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2">
+        <v>50</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="2">
+        <v>15</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="K31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="2">
+        <v>50</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" s="6" t="s">
+    </row>
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="H39" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+    </row>
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K26" s="6">
+      <c r="E44" s="2">
+        <v>100</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H46" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="H53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="H54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+    </row>
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="H55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+    </row>
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="7"/>
+      <c r="H56" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+    </row>
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="C59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="2">
+        <v>50</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L27" s="6" t="s">
+      <c r="H59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K59" s="2">
+        <v>50</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H28" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K28" s="6">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K60" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L28" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H29" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="6">
-        <v>50</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H30" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="6">
-        <v>15</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H31" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J31" s="6" t="s">
+      <c r="E71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H32" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="6">
-        <v>50</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H33" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H34" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J34" s="6" t="s">
+      <c r="E72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="11"/>
-      <c r="H39" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-    </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-    </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-    </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="6">
-        <v>100</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="8" t="s">
+      <c r="E73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L44" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H45" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H46" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="H53" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-    </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="H54" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-    </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="H55" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-    </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="11"/>
-      <c r="H56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-    </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L57" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I58" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K58" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L58" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E59" s="6">
-        <v>50</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H59" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K59" s="6">
-        <v>50</v>
-      </c>
-      <c r="L59" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I60" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K60" s="6">
-        <v>5.2</v>
-      </c>
-      <c r="L60" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E61" s="6">
-        <v>5.2</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B69" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B71" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B72" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B73" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H56:L56"/>
-    <mergeCell ref="C67:F67"/>
-    <mergeCell ref="C68:F68"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="I53:L53"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="I55:L55"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="I20:L20"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="I40:L40"/>
     <mergeCell ref="C38:F38"/>
@@ -2259,18 +2239,17 @@
     <mergeCell ref="H22:L22"/>
     <mergeCell ref="C36:F36"/>
     <mergeCell ref="I39:L39"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="I53:L53"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="I55:L55"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B70:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>